<commit_message>
Cambio PID - Resta 1.9s
</commit_message>
<xml_diff>
--- a/Laboratorio6-CinematicaMovil/ControlAndPoseEstimationAnalysis.xlsx
+++ b/Laboratorio6-CinematicaMovil/ControlAndPoseEstimationAnalysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agurt\OneDrive\CICLO 24-2\ROBÓTICA E INTELIGENCIA ARTIFICIAL\Laboratorios\Laboratorio6\Laboratorio6-CinematicaMovil\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/981e0c618f971599/1. Católica Archivos (2024-2)/Robótica e Inteligencia Artificial/Laboratorio 6/Laboratorio6/Laboratorio6-CinematicaMovil/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3FD35BC-268F-4EBD-ADE6-B1516E81843B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="13_ncr:1_{D3FD35BC-268F-4EBD-ADE6-B1516E81843B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B960720E-05C6-4D01-999E-F9782DD49713}"/>
   <bookViews>
-    <workbookView xWindow="20660" yWindow="840" windowWidth="17280" windowHeight="8980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="P2" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="35">
   <si>
     <t>Colocar aquí los resultados y gráficas de la segunda pregunta</t>
   </si>
@@ -131,6 +131,15 @@
   <si>
     <t>Td</t>
   </si>
+  <si>
+    <t>MOTOR 2</t>
+  </si>
+  <si>
+    <t>MOTOR 1</t>
+  </si>
+  <si>
+    <t>Tiempo escalón lanzar</t>
+  </si>
 </sst>
 </file>
 
@@ -211,7 +220,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -312,11 +321,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -337,25 +355,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
@@ -364,6 +363,31 @@
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -384,7 +408,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -720,7 +744,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1070,7 +1094,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1406,7 +1430,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4598,19 +4622,25 @@
   </sheetPr>
   <dimension ref="A2:N166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K47" sqref="K47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="8" t="s">
+      <c r="G2" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="8">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B5" s="14" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -4622,24 +4652,27 @@
       <c r="E5" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="9"/>
+      <c r="G5" s="23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B6" s="15"/>
       <c r="C6" s="3">
         <f>K50</f>
-        <v>8.5279187817258822E-2</v>
+        <v>2.3999999999999959</v>
       </c>
       <c r="D6" s="3">
         <f>K51</f>
-        <v>2.1644463913009854E-2</v>
+        <v>17.1428571428571</v>
       </c>
       <c r="E6" s="3">
         <f>K52</f>
         <v>8.3999999999999936E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="8" t="s">
+    <row r="8" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B8" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -4651,24 +4684,27 @@
       <c r="E8" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="9"/>
+      <c r="G8" s="23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B9" s="15"/>
       <c r="C9" s="3">
         <f>K90</f>
-        <v>9.1836734693877486E-2</v>
+        <v>2.9999999999999956</v>
       </c>
       <c r="D9" s="3">
         <f>K91</f>
-        <v>2.3427738442315684E-2</v>
+        <v>24.99999999999994</v>
       </c>
       <c r="E9" s="3">
         <f>K92</f>
         <v>8.9999999999999941E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="8" t="s">
+    <row r="11" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B11" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -4681,23 +4717,23 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="9"/>
+    <row r="12" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B12" s="15"/>
       <c r="C12" s="3">
         <f>K125</f>
-        <v>8.5279187817258822E-2</v>
+        <v>2.3999999999999959</v>
       </c>
       <c r="D12" s="3">
         <f>K126</f>
-        <v>2.1644463913009854E-2</v>
+        <v>17.1428571428571</v>
       </c>
       <c r="E12" s="3">
         <f>K127</f>
         <v>8.3999999999999936E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="8" t="s">
+    <row r="14" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B14" s="14" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -4710,41 +4746,41 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="9"/>
+    <row r="15" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B15" s="15"/>
       <c r="C15" s="3">
         <f>K164</f>
-        <v>7.9187817258883325E-2</v>
+        <v>2.2285714285714286</v>
       </c>
       <c r="D15" s="3">
         <f>K165</f>
-        <v>2.0098430776366326E-2</v>
+        <v>15.918367346938762</v>
       </c>
       <c r="E15" s="3">
         <f>K166</f>
         <v>7.8000000000000069E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C38" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D39" s="17" t="s">
+    <row r="39" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D39" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E39" s="17" t="s">
+      <c r="E39" s="8" t="s">
         <v>23</v>
       </c>
       <c r="I39" t="s">
@@ -4755,11 +4791,11 @@
         <v>655.17999999999995</v>
       </c>
     </row>
-    <row r="40" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D40" s="17">
+    <row r="40" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D40" s="8">
         <v>2.0505200000000001</v>
       </c>
-      <c r="E40" s="17">
+      <c r="E40" s="8">
         <v>53.5</v>
       </c>
       <c r="I40" t="s">
@@ -4769,29 +4805,29 @@
         <v>-1290</v>
       </c>
     </row>
-    <row r="41" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D41" s="17">
+    <row r="41" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D41" s="8">
         <v>2.100552</v>
       </c>
-      <c r="E41" s="17">
+      <c r="E41" s="8">
         <v>86.28</v>
       </c>
     </row>
-    <row r="43" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I43" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J44" s="18" t="s">
+    <row r="44" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J44" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="K44" s="18">
-        <f>-ROUND(J40/J39,2)</f>
-        <v>1.97</v>
-      </c>
-    </row>
-    <row r="46" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K44" s="9">
+        <f>-ROUND(J40/J39,2) - H2</f>
+        <v>7.0000000000000062E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I46" t="s">
         <v>28</v>
       </c>
@@ -4799,85 +4835,85 @@
         <v>90.61</v>
       </c>
     </row>
-    <row r="47" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J47" t="s">
         <v>22</v>
       </c>
       <c r="K47">
-        <f>ROUND((J46-J40)/J39,2)</f>
-        <v>2.11</v>
-      </c>
-    </row>
-    <row r="48" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J48" s="18" t="s">
+        <f>ROUND((J46-J40)/J39,2) -H2</f>
+        <v>0.20999999999999996</v>
+      </c>
+    </row>
+    <row r="48" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J48" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="K48" s="18">
+      <c r="K48" s="9">
         <f>K47-K44</f>
         <v>0.1399999999999999</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J50" s="19" t="s">
+    <row r="50" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J50" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="K50" s="19">
+      <c r="K50" s="10">
         <f>1.2*K48/K44</f>
-        <v>8.5279187817258822E-2</v>
-      </c>
-      <c r="M50" s="20" t="s">
+        <v>2.3999999999999959</v>
+      </c>
+      <c r="M50" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="N50" s="20">
+      <c r="N50" s="11">
         <f>2*K44</f>
-        <v>3.94</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J51" s="19" t="s">
+        <v>0.14000000000000012</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J51" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="K51" s="19">
+      <c r="K51" s="10">
         <f>K50/N50</f>
-        <v>2.1644463913009854E-2</v>
-      </c>
-      <c r="M51" s="20" t="s">
+        <v>17.1428571428571</v>
+      </c>
+      <c r="M51" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="N51" s="20">
+      <c r="N51" s="11">
         <f>0.5*K44</f>
-        <v>0.98499999999999999</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J52" s="19" t="s">
+        <v>3.5000000000000031E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J52" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="K52" s="19">
+      <c r="K52" s="10">
         <f>K50*N51</f>
         <v>8.3999999999999936E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="78" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C78" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="79" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D79" s="17" t="s">
+    <row r="79" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D79" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E79" s="17" t="s">
+      <c r="E79" s="8" t="s">
         <v>23</v>
       </c>
       <c r="I79" t="s">
@@ -4887,43 +4923,43 @@
         <v>586.41</v>
       </c>
     </row>
-    <row r="80" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D80" s="17">
+    <row r="80" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D80" s="8">
         <v>2.0505080000000002</v>
       </c>
-      <c r="E80" s="17">
+      <c r="E80" s="8">
         <v>54.38</v>
       </c>
       <c r="I80" t="s">
         <v>25</v>
       </c>
-      <c r="J80" s="21">
+      <c r="J80" s="12">
         <v>-1148.0999999999999</v>
       </c>
     </row>
-    <row r="81" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D81" s="17">
+    <row r="81" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D81" s="8">
         <v>2.1005240000000001</v>
       </c>
-      <c r="E81" s="17">
+      <c r="E81" s="8">
         <v>83.71</v>
       </c>
     </row>
-    <row r="83" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I83" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="84" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J84" s="18" t="s">
+    <row r="84" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J84" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="K84" s="18">
-        <f>-ROUND(J80/J79,2)</f>
-        <v>1.96</v>
-      </c>
-    </row>
-    <row r="86" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K84" s="9">
+        <f>-ROUND(J80/J79,2) - H2</f>
+        <v>6.0000000000000053E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I86" t="s">
         <v>28</v>
       </c>
@@ -4931,85 +4967,85 @@
         <v>88.89</v>
       </c>
     </row>
-    <row r="87" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J87" t="s">
         <v>22</v>
       </c>
       <c r="K87">
-        <f>ROUND((J86-J80)/J79,2)</f>
-        <v>2.11</v>
-      </c>
-    </row>
-    <row r="88" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J88" s="18" t="s">
+        <f>ROUND((J86-J80)/J79,2) - H2</f>
+        <v>0.20999999999999996</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J88" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="K88" s="18">
+      <c r="K88" s="9">
         <f>K87-K84</f>
         <v>0.14999999999999991</v>
       </c>
     </row>
-    <row r="90" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J90" s="19" t="s">
+    <row r="90" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J90" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="K90" s="19">
+      <c r="K90" s="10">
         <f>1.2*K88/K84</f>
-        <v>9.1836734693877486E-2</v>
-      </c>
-      <c r="M90" s="20" t="s">
+        <v>2.9999999999999956</v>
+      </c>
+      <c r="M90" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="N90" s="20">
+      <c r="N90" s="11">
         <f>2*K84</f>
-        <v>3.92</v>
-      </c>
-    </row>
-    <row r="91" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J91" s="19" t="s">
+        <v>0.12000000000000011</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J91" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="K91" s="19">
+      <c r="K91" s="10">
         <f>K90/N90</f>
-        <v>2.3427738442315684E-2</v>
-      </c>
-      <c r="M91" s="20" t="s">
+        <v>24.99999999999994</v>
+      </c>
+      <c r="M91" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="N91" s="20">
+      <c r="N91" s="11">
         <f>0.5*K84</f>
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="92" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J92" s="19" t="s">
+        <v>3.0000000000000027E-2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J92" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="K92" s="19">
+      <c r="K92" s="10">
         <f>K90*N91</f>
         <v>8.9999999999999941E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="22" t="s">
+    <row r="94" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="111" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B111" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="113" spans="3:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="3:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C113" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="114" spans="3:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D114" s="17" t="s">
+    <row r="114" spans="3:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D114" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E114" s="17" t="s">
+      <c r="E114" s="8" t="s">
         <v>23</v>
       </c>
       <c r="I114" t="s">
@@ -5019,43 +5055,43 @@
         <v>638.75</v>
       </c>
     </row>
-    <row r="115" spans="3:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D115" s="17">
+    <row r="115" spans="3:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D115" s="8">
         <v>2.0505040000000001</v>
       </c>
-      <c r="E115" s="17">
+      <c r="E115" s="8">
         <v>54.38</v>
       </c>
       <c r="I115" t="s">
         <v>25</v>
       </c>
-      <c r="J115" s="21">
+      <c r="J115" s="12">
         <v>-1255.4000000000001</v>
       </c>
     </row>
-    <row r="116" spans="3:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D116" s="17">
+    <row r="116" spans="3:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D116" s="8">
         <v>2.100508</v>
       </c>
-      <c r="E116" s="17">
+      <c r="E116" s="8">
         <v>86.32</v>
       </c>
     </row>
-    <row r="118" spans="3:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="3:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I118" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="119" spans="3:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J119" s="18" t="s">
+    <row r="119" spans="3:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J119" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="K119" s="18">
-        <f>-ROUND(J115/J114,2)</f>
-        <v>1.97</v>
-      </c>
-    </row>
-    <row r="121" spans="3:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K119" s="9">
+        <f>-ROUND(J115/J114,2) - H2</f>
+        <v>7.0000000000000062E-2</v>
+      </c>
+    </row>
+    <row r="121" spans="3:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I121" t="s">
         <v>28</v>
       </c>
@@ -5063,85 +5099,85 @@
         <v>91.5</v>
       </c>
     </row>
-    <row r="122" spans="3:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="3:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J122" t="s">
         <v>22</v>
       </c>
       <c r="K122">
-        <f>ROUND((J121-J115)/J114,2)</f>
-        <v>2.11</v>
-      </c>
-    </row>
-    <row r="123" spans="3:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J123" s="18" t="s">
+        <f>ROUND((J121-J115)/J114,2) - H2</f>
+        <v>0.20999999999999996</v>
+      </c>
+    </row>
+    <row r="123" spans="3:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J123" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="K123" s="18">
+      <c r="K123" s="9">
         <f>K122-K119</f>
         <v>0.1399999999999999</v>
       </c>
     </row>
-    <row r="125" spans="3:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J125" s="19" t="s">
+    <row r="125" spans="3:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J125" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="K125" s="19">
+      <c r="K125" s="10">
         <f>1.2*K123/K119</f>
-        <v>8.5279187817258822E-2</v>
-      </c>
-      <c r="M125" s="20" t="s">
+        <v>2.3999999999999959</v>
+      </c>
+      <c r="M125" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="N125" s="20">
+      <c r="N125" s="11">
         <f>2*K119</f>
-        <v>3.94</v>
-      </c>
-    </row>
-    <row r="126" spans="3:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J126" s="19" t="s">
+        <v>0.14000000000000012</v>
+      </c>
+    </row>
+    <row r="126" spans="3:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J126" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="K126" s="19">
+      <c r="K126" s="10">
         <f>K125/N125</f>
-        <v>2.1644463913009854E-2</v>
-      </c>
-      <c r="M126" s="20" t="s">
+        <v>17.1428571428571</v>
+      </c>
+      <c r="M126" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="N126" s="20">
+      <c r="N126" s="11">
         <f>0.5*K119</f>
-        <v>0.98499999999999999</v>
-      </c>
-    </row>
-    <row r="127" spans="3:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J127" s="19" t="s">
+        <v>3.5000000000000031E-2</v>
+      </c>
+    </row>
+    <row r="127" spans="3:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J127" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="K127" s="19">
+      <c r="K127" s="10">
         <f>K125*N126</f>
         <v>8.3999999999999936E-2</v>
       </c>
     </row>
-    <row r="132" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="22" t="s">
+    <row r="132" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A132" s="13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="150" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B150" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="152" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C152" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="153" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D153" s="17" t="s">
+    <row r="153" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D153" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E153" s="17" t="s">
+      <c r="E153" s="8" t="s">
         <v>23</v>
       </c>
       <c r="I153" t="s">
@@ -5151,11 +5187,11 @@
         <v>656.04</v>
       </c>
     </row>
-    <row r="154" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D154" s="17">
+    <row r="154" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D154" s="8">
         <v>2.0505200000000001</v>
       </c>
-      <c r="E154" s="17">
+      <c r="E154" s="8">
         <v>54.36</v>
       </c>
       <c r="I154" t="s">
@@ -5165,29 +5201,29 @@
         <v>-1290.9000000000001</v>
       </c>
     </row>
-    <row r="155" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D155" s="17">
+    <row r="155" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D155" s="8">
         <v>2.1005319999999998</v>
       </c>
-      <c r="E155" s="17">
+      <c r="E155" s="8">
         <v>87.17</v>
       </c>
     </row>
-    <row r="157" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I157" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="158" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J158" s="18" t="s">
+    <row r="158" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J158" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="K158" s="18">
-        <f>-ROUND(J154/J153,2)</f>
-        <v>1.97</v>
-      </c>
-    </row>
-    <row r="160" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K158" s="9">
+        <f>-ROUND(J154/J153,2) - H2</f>
+        <v>7.0000000000000062E-2</v>
+      </c>
+    </row>
+    <row r="160" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I160" t="s">
         <v>28</v>
       </c>
@@ -5195,61 +5231,61 @@
         <v>88.89</v>
       </c>
     </row>
-    <row r="161" spans="10:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="10:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J161" t="s">
         <v>22</v>
       </c>
       <c r="K161">
-        <f>ROUND((J160-J154)/J153,2)</f>
-        <v>2.1</v>
-      </c>
-    </row>
-    <row r="162" spans="10:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J162" s="18" t="s">
+        <f>ROUND((J160-J154)/J153,2)-H2</f>
+        <v>0.20000000000000018</v>
+      </c>
+    </row>
+    <row r="162" spans="10:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J162" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="K162" s="18">
+      <c r="K162" s="9">
         <f>K161-K158</f>
         <v>0.13000000000000012</v>
       </c>
     </row>
-    <row r="164" spans="10:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J164" s="19" t="s">
+    <row r="164" spans="10:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J164" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="K164" s="19">
+      <c r="K164" s="10">
         <f>1.2*K162/K158</f>
-        <v>7.9187817258883325E-2</v>
-      </c>
-      <c r="M164" s="20" t="s">
+        <v>2.2285714285714286</v>
+      </c>
+      <c r="M164" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="N164" s="20">
+      <c r="N164" s="11">
         <f>2*K158</f>
-        <v>3.94</v>
-      </c>
-    </row>
-    <row r="165" spans="10:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J165" s="19" t="s">
+        <v>0.14000000000000012</v>
+      </c>
+    </row>
+    <row r="165" spans="10:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J165" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="K165" s="19">
+      <c r="K165" s="10">
         <f>K164/N164</f>
-        <v>2.0098430776366326E-2</v>
-      </c>
-      <c r="M165" s="20" t="s">
+        <v>15.918367346938762</v>
+      </c>
+      <c r="M165" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="N165" s="20">
+      <c r="N165" s="11">
         <f>0.5*K158</f>
-        <v>0.98499999999999999</v>
-      </c>
-    </row>
-    <row r="166" spans="10:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J166" s="19" t="s">
+        <v>3.5000000000000031E-2</v>
+      </c>
+    </row>
+    <row r="166" spans="10:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J166" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="K166" s="19">
+      <c r="K166" s="10">
         <f>K164*N165</f>
         <v>7.8000000000000069E-2</v>
       </c>
@@ -5275,37 +5311,37 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="7" width="10" customWidth="1"/>
-    <col min="8" max="10" width="11.109375" customWidth="1"/>
+    <col min="8" max="10" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="10" t="s">
+    <row r="3" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="13" t="s">
+      <c r="D3" s="18"/>
+      <c r="E3" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="14"/>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="9"/>
+      <c r="I3" s="16"/>
+    </row>
+    <row r="4" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="15"/>
       <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="9"/>
-      <c r="I4" s="14"/>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="E4" s="15"/>
+      <c r="I4" s="16"/>
+    </row>
+    <row r="5" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="5" t="s">
         <v>13</v>
       </c>
@@ -5316,7 +5352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
         <v>14</v>
       </c>
@@ -5327,7 +5363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="5" t="s">
         <v>15</v>
       </c>
@@ -5338,40 +5374,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="10" t="s">
+    <row r="9" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="13" t="s">
+      <c r="D9" s="18"/>
+      <c r="E9" s="19" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="9"/>
+    <row r="10" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="15"/>
       <c r="C10" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="9"/>
-      <c r="H10" s="15" t="s">
+      <c r="E10" s="15"/>
+      <c r="H10" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="I10" s="16"/>
-      <c r="J10" s="12"/>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I10" s="21"/>
+      <c r="J10" s="18"/>
+    </row>
+    <row r="11" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="5" t="s">
         <v>13</v>
       </c>
@@ -5391,7 +5427,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="5" t="s">
         <v>14</v>
       </c>
@@ -5414,7 +5450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="5" t="s">
         <v>15</v>
       </c>
@@ -5425,35 +5461,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="10" t="s">
+    <row r="15" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="12"/>
-      <c r="E15" s="13" t="s">
+      <c r="D15" s="18"/>
+      <c r="E15" s="19" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="9"/>
+    <row r="16" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="15"/>
       <c r="C16" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="9"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E16" s="15"/>
+    </row>
+    <row r="17" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="5" t="s">
         <v>13</v>
       </c>
@@ -5464,7 +5500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="5" t="s">
         <v>14</v>
       </c>
@@ -5475,7 +5511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="5" t="s">
         <v>15</v>
       </c>
@@ -5486,24 +5522,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="B9:B10"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="E15:E16"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:E4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="B9:B10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Se agrego archivos de Rodrigo y Jairo
</commit_message>
<xml_diff>
--- a/Laboratorio6-CinematicaMovil/ControlAndPoseEstimationAnalysis.xlsx
+++ b/Laboratorio6-CinematicaMovil/ControlAndPoseEstimationAnalysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/981e0c618f971599/1. Católica Archivos (2024-2)/Robótica e Inteligencia Artificial/Laboratorio 6/Laboratorio6/Laboratorio6-CinematicaMovil/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PREDATOR\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="13_ncr:1_{D3FD35BC-268F-4EBD-ADE6-B1516E81843B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B960720E-05C6-4D01-999E-F9782DD49713}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53405F45-C911-4923-9C1F-AA801CFD15B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="P2" sheetId="1" r:id="rId1"/>
@@ -25,8 +25,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -363,11 +361,19 @@
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -375,19 +381,11 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,7 +443,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-PE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -519,7 +517,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="es-PE"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -627,7 +625,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-PE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="718384031"/>
@@ -689,7 +687,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-PE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="718381151"/>
@@ -730,7 +728,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-PE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -781,7 +779,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-PE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -869,7 +867,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="es-PE"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -977,7 +975,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-PE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="955762335"/>
@@ -1039,7 +1037,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-PE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="955758975"/>
@@ -1080,7 +1078,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-PE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1131,7 +1129,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-PE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1205,7 +1203,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="es-PE"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1313,7 +1311,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-PE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="955758975"/>
@@ -1375,7 +1373,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-PE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="955760895"/>
@@ -1416,7 +1414,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-PE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1467,7 +1465,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-PE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1541,7 +1539,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="es-PE"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1649,7 +1647,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-PE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="718386431"/>
@@ -1711,7 +1709,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-PE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="718388351"/>
@@ -1752,7 +1750,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-PE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4622,25 +4620,25 @@
   </sheetPr>
   <dimension ref="A2:N166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K47" sqref="K47"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="G2" s="15" t="s">
         <v>34</v>
       </c>
       <c r="H2" s="8">
-        <v>1.9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B5" s="14" t="s">
+        <v>1.85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B5" s="16" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -4652,27 +4650,27 @@
       <c r="E5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="23" t="s">
+      <c r="G5" s="14" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B6" s="15"/>
+    <row r="6" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B6" s="17"/>
       <c r="C6" s="3">
         <f>K50</f>
-        <v>2.3999999999999959</v>
+        <v>1.4000000000000004</v>
       </c>
       <c r="D6" s="3">
         <f>K51</f>
-        <v>17.1428571428571</v>
+        <v>5.8333333333333401</v>
       </c>
       <c r="E6" s="3">
         <f>K52</f>
         <v>8.3999999999999936E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B8" s="14" t="s">
+    <row r="8" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B8" s="16" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -4684,27 +4682,27 @@
       <c r="E8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="23" t="s">
+      <c r="G8" s="14" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B9" s="15"/>
+    <row r="9" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B9" s="17"/>
       <c r="C9" s="3">
         <f>K90</f>
-        <v>2.9999999999999956</v>
+        <v>1.6363636363636371</v>
       </c>
       <c r="D9" s="3">
         <f>K91</f>
-        <v>24.99999999999994</v>
+        <v>7.4380165289256315</v>
       </c>
       <c r="E9" s="3">
         <f>K92</f>
         <v>8.9999999999999941E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B11" s="14" t="s">
+    <row r="11" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B11" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -4717,23 +4715,23 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B12" s="15"/>
+    <row r="12" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B12" s="17"/>
       <c r="C12" s="3">
         <f>K125</f>
-        <v>2.3999999999999959</v>
+        <v>1.4000000000000004</v>
       </c>
       <c r="D12" s="3">
         <f>K126</f>
-        <v>17.1428571428571</v>
+        <v>5.8333333333333401</v>
       </c>
       <c r="E12" s="3">
         <f>K127</f>
         <v>8.3999999999999936E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B14" s="14" t="s">
+    <row r="14" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B14" s="16" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -4746,37 +4744,37 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B15" s="15"/>
+    <row r="15" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B15" s="17"/>
       <c r="C15" s="3">
         <f>K164</f>
-        <v>2.2285714285714286</v>
+        <v>1.3000000000000025</v>
       </c>
       <c r="D15" s="3">
         <f>K165</f>
-        <v>15.918367346938762</v>
+        <v>5.4166666666666821</v>
       </c>
       <c r="E15" s="3">
         <f>K166</f>
         <v>7.8000000000000069E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D39" s="8" t="s">
         <v>22</v>
       </c>
@@ -4791,7 +4789,7 @@
         <v>655.17999999999995</v>
       </c>
     </row>
-    <row r="40" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D40" s="8">
         <v>2.0505200000000001</v>
       </c>
@@ -4805,7 +4803,7 @@
         <v>-1290</v>
       </c>
     </row>
-    <row r="41" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D41" s="8">
         <v>2.100552</v>
       </c>
@@ -4813,21 +4811,21 @@
         <v>86.28</v>
       </c>
     </row>
-    <row r="43" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I43" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J44" s="9" t="s">
         <v>27</v>
       </c>
       <c r="K44" s="9">
         <f>-ROUND(J40/J39,2) - H2</f>
-        <v>7.0000000000000062E-2</v>
-      </c>
-    </row>
-    <row r="46" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0.11999999999999988</v>
+      </c>
+    </row>
+    <row r="46" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I46" t="s">
         <v>28</v>
       </c>
@@ -4835,16 +4833,16 @@
         <v>90.61</v>
       </c>
     </row>
-    <row r="47" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J47" t="s">
         <v>22</v>
       </c>
       <c r="K47">
         <f>ROUND((J46-J40)/J39,2) -H2</f>
-        <v>0.20999999999999996</v>
-      </c>
-    </row>
-    <row r="48" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0.25999999999999979</v>
+      </c>
+    </row>
+    <row r="48" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J48" s="9" t="s">
         <v>29</v>
       </c>
@@ -4853,39 +4851,39 @@
         <v>0.1399999999999999</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J50" s="10" t="s">
         <v>2</v>
       </c>
       <c r="K50" s="10">
         <f>1.2*K48/K44</f>
-        <v>2.3999999999999959</v>
+        <v>1.4000000000000004</v>
       </c>
       <c r="M50" s="11" t="s">
         <v>30</v>
       </c>
       <c r="N50" s="11">
         <f>2*K44</f>
-        <v>0.14000000000000012</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0.23999999999999977</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J51" s="10" t="s">
         <v>3</v>
       </c>
       <c r="K51" s="10">
         <f>K50/N50</f>
-        <v>17.1428571428571</v>
+        <v>5.8333333333333401</v>
       </c>
       <c r="M51" s="11" t="s">
         <v>31</v>
       </c>
       <c r="N51" s="11">
         <f>0.5*K44</f>
-        <v>3.5000000000000031E-2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>5.9999999999999942E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J52" s="10" t="s">
         <v>4</v>
       </c>
@@ -4894,22 +4892,22 @@
         <v>8.3999999999999936E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="78" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C78" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="79" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D79" s="8" t="s">
         <v>22</v>
       </c>
@@ -4923,7 +4921,7 @@
         <v>586.41</v>
       </c>
     </row>
-    <row r="80" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D80" s="8">
         <v>2.0505080000000002</v>
       </c>
@@ -4937,7 +4935,7 @@
         <v>-1148.0999999999999</v>
       </c>
     </row>
-    <row r="81" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D81" s="8">
         <v>2.1005240000000001</v>
       </c>
@@ -4945,21 +4943,21 @@
         <v>83.71</v>
       </c>
     </row>
-    <row r="83" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I83" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="84" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J84" s="9" t="s">
         <v>27</v>
       </c>
       <c r="K84" s="9">
         <f>-ROUND(J80/J79,2) - H2</f>
-        <v>6.0000000000000053E-2</v>
-      </c>
-    </row>
-    <row r="86" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0.10999999999999988</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I86" t="s">
         <v>28</v>
       </c>
@@ -4967,16 +4965,16 @@
         <v>88.89</v>
       </c>
     </row>
-    <row r="87" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J87" t="s">
         <v>22</v>
       </c>
       <c r="K87">
         <f>ROUND((J86-J80)/J79,2) - H2</f>
-        <v>0.20999999999999996</v>
-      </c>
-    </row>
-    <row r="88" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0.25999999999999979</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J88" s="9" t="s">
         <v>29</v>
       </c>
@@ -4985,39 +4983,39 @@
         <v>0.14999999999999991</v>
       </c>
     </row>
-    <row r="90" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J90" s="10" t="s">
         <v>2</v>
       </c>
       <c r="K90" s="10">
         <f>1.2*K88/K84</f>
-        <v>2.9999999999999956</v>
+        <v>1.6363636363636371</v>
       </c>
       <c r="M90" s="11" t="s">
         <v>30</v>
       </c>
       <c r="N90" s="11">
         <f>2*K84</f>
-        <v>0.12000000000000011</v>
-      </c>
-    </row>
-    <row r="91" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0.21999999999999975</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J91" s="10" t="s">
         <v>3</v>
       </c>
       <c r="K91" s="10">
         <f>K90/N90</f>
-        <v>24.99999999999994</v>
+        <v>7.4380165289256315</v>
       </c>
       <c r="M91" s="11" t="s">
         <v>31</v>
       </c>
       <c r="N91" s="11">
         <f>0.5*K84</f>
-        <v>3.0000000000000027E-2</v>
-      </c>
-    </row>
-    <row r="92" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>5.4999999999999938E-2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J92" s="10" t="s">
         <v>4</v>
       </c>
@@ -5026,22 +5024,22 @@
         <v>8.9999999999999941E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="111" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="113" spans="3:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="3:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C113" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="114" spans="3:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="3:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D114" s="8" t="s">
         <v>22</v>
       </c>
@@ -5055,7 +5053,7 @@
         <v>638.75</v>
       </c>
     </row>
-    <row r="115" spans="3:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="3:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D115" s="8">
         <v>2.0505040000000001</v>
       </c>
@@ -5069,7 +5067,7 @@
         <v>-1255.4000000000001</v>
       </c>
     </row>
-    <row r="116" spans="3:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="3:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D116" s="8">
         <v>2.100508</v>
       </c>
@@ -5077,21 +5075,21 @@
         <v>86.32</v>
       </c>
     </row>
-    <row r="118" spans="3:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="3:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I118" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="119" spans="3:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="3:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J119" s="9" t="s">
         <v>27</v>
       </c>
       <c r="K119" s="9">
         <f>-ROUND(J115/J114,2) - H2</f>
-        <v>7.0000000000000062E-2</v>
-      </c>
-    </row>
-    <row r="121" spans="3:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0.11999999999999988</v>
+      </c>
+    </row>
+    <row r="121" spans="3:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I121" t="s">
         <v>28</v>
       </c>
@@ -5099,16 +5097,16 @@
         <v>91.5</v>
       </c>
     </row>
-    <row r="122" spans="3:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="3:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J122" t="s">
         <v>22</v>
       </c>
       <c r="K122">
         <f>ROUND((J121-J115)/J114,2) - H2</f>
-        <v>0.20999999999999996</v>
-      </c>
-    </row>
-    <row r="123" spans="3:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0.25999999999999979</v>
+      </c>
+    </row>
+    <row r="123" spans="3:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J123" s="9" t="s">
         <v>29</v>
       </c>
@@ -5117,39 +5115,39 @@
         <v>0.1399999999999999</v>
       </c>
     </row>
-    <row r="125" spans="3:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="3:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J125" s="10" t="s">
         <v>2</v>
       </c>
       <c r="K125" s="10">
         <f>1.2*K123/K119</f>
-        <v>2.3999999999999959</v>
+        <v>1.4000000000000004</v>
       </c>
       <c r="M125" s="11" t="s">
         <v>30</v>
       </c>
       <c r="N125" s="11">
         <f>2*K119</f>
-        <v>0.14000000000000012</v>
-      </c>
-    </row>
-    <row r="126" spans="3:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0.23999999999999977</v>
+      </c>
+    </row>
+    <row r="126" spans="3:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J126" s="10" t="s">
         <v>3</v>
       </c>
       <c r="K126" s="10">
         <f>K125/N125</f>
-        <v>17.1428571428571</v>
+        <v>5.8333333333333401</v>
       </c>
       <c r="M126" s="11" t="s">
         <v>31</v>
       </c>
       <c r="N126" s="11">
         <f>0.5*K119</f>
-        <v>3.5000000000000031E-2</v>
-      </c>
-    </row>
-    <row r="127" spans="3:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>5.9999999999999942E-2</v>
+      </c>
+    </row>
+    <row r="127" spans="3:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J127" s="10" t="s">
         <v>4</v>
       </c>
@@ -5158,22 +5156,22 @@
         <v>8.3999999999999936E-2</v>
       </c>
     </row>
-    <row r="132" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="150" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B150" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="152" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C152" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="153" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D153" s="8" t="s">
         <v>22</v>
       </c>
@@ -5187,7 +5185,7 @@
         <v>656.04</v>
       </c>
     </row>
-    <row r="154" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D154" s="8">
         <v>2.0505200000000001</v>
       </c>
@@ -5201,7 +5199,7 @@
         <v>-1290.9000000000001</v>
       </c>
     </row>
-    <row r="155" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D155" s="8">
         <v>2.1005319999999998</v>
       </c>
@@ -5209,21 +5207,21 @@
         <v>87.17</v>
       </c>
     </row>
-    <row r="157" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I157" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="158" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J158" s="9" t="s">
         <v>27</v>
       </c>
       <c r="K158" s="9">
         <f>-ROUND(J154/J153,2) - H2</f>
-        <v>7.0000000000000062E-2</v>
-      </c>
-    </row>
-    <row r="160" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0.11999999999999988</v>
+      </c>
+    </row>
+    <row r="160" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I160" t="s">
         <v>28</v>
       </c>
@@ -5231,16 +5229,16 @@
         <v>88.89</v>
       </c>
     </row>
-    <row r="161" spans="10:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="10:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J161" t="s">
         <v>22</v>
       </c>
       <c r="K161">
         <f>ROUND((J160-J154)/J153,2)-H2</f>
-        <v>0.20000000000000018</v>
-      </c>
-    </row>
-    <row r="162" spans="10:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="162" spans="10:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J162" s="9" t="s">
         <v>29</v>
       </c>
@@ -5249,39 +5247,39 @@
         <v>0.13000000000000012</v>
       </c>
     </row>
-    <row r="164" spans="10:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="10:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J164" s="10" t="s">
         <v>2</v>
       </c>
       <c r="K164" s="10">
         <f>1.2*K162/K158</f>
-        <v>2.2285714285714286</v>
+        <v>1.3000000000000025</v>
       </c>
       <c r="M164" s="11" t="s">
         <v>30</v>
       </c>
       <c r="N164" s="11">
         <f>2*K158</f>
-        <v>0.14000000000000012</v>
-      </c>
-    </row>
-    <row r="165" spans="10:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0.23999999999999977</v>
+      </c>
+    </row>
+    <row r="165" spans="10:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J165" s="10" t="s">
         <v>3</v>
       </c>
       <c r="K165" s="10">
         <f>K164/N164</f>
-        <v>15.918367346938762</v>
+        <v>5.4166666666666821</v>
       </c>
       <c r="M165" s="11" t="s">
         <v>31</v>
       </c>
       <c r="N165" s="11">
         <f>0.5*K158</f>
-        <v>3.5000000000000031E-2</v>
-      </c>
-    </row>
-    <row r="166" spans="10:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>5.9999999999999942E-2</v>
+      </c>
+    </row>
+    <row r="166" spans="10:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J166" s="10" t="s">
         <v>4</v>
       </c>
@@ -5311,37 +5309,37 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="7" width="10" customWidth="1"/>
-    <col min="8" max="10" width="11.140625" customWidth="1"/>
+    <col min="8" max="10" width="11.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="22" t="s">
+    <row r="3" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="19" t="s">
+      <c r="D3" s="20"/>
+      <c r="E3" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="16"/>
-    </row>
-    <row r="4" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="15"/>
+      <c r="I3" s="22"/>
+    </row>
+    <row r="4" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="17"/>
       <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="15"/>
-      <c r="I4" s="16"/>
-    </row>
-    <row r="5" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E4" s="17"/>
+      <c r="I4" s="22"/>
+    </row>
+    <row r="5" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>13</v>
       </c>
@@ -5352,7 +5350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>14</v>
       </c>
@@ -5363,7 +5361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>15</v>
       </c>
@@ -5374,40 +5372,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
     </row>
-    <row r="9" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="22" t="s">
+    <row r="9" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="19" t="s">
+      <c r="D9" s="20"/>
+      <c r="E9" s="21" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="15"/>
+    <row r="10" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="17"/>
       <c r="C10" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="15"/>
-      <c r="H10" s="20" t="s">
+      <c r="E10" s="17"/>
+      <c r="H10" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="I10" s="21"/>
-      <c r="J10" s="18"/>
-    </row>
-    <row r="11" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I10" s="24"/>
+      <c r="J10" s="20"/>
+    </row>
+    <row r="11" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>13</v>
       </c>
@@ -5427,7 +5425,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>14</v>
       </c>
@@ -5450,7 +5448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>15</v>
       </c>
@@ -5461,35 +5459,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
     </row>
-    <row r="15" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="22" t="s">
+    <row r="15" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="19" t="s">
+      <c r="D15" s="20"/>
+      <c r="E15" s="21" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="15"/>
+    <row r="16" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="17"/>
       <c r="C16" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="15"/>
-    </row>
-    <row r="17" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E16" s="17"/>
+    </row>
+    <row r="17" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>13</v>
       </c>
@@ -5500,7 +5498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>14</v>
       </c>
@@ -5511,7 +5509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>15</v>
       </c>
@@ -5522,24 +5520,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="B9:B10"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="E15:E16"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:E4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="B9:B10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>